<commit_message>
Actualización num. 2 150316
</commit_message>
<xml_diff>
--- a/ACT/IPT_ReunionesTema5y6_150316.xlsx
+++ b/ACT/IPT_ReunionesTema5y6_150316.xlsx
@@ -162,7 +162,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\-m\-yy;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,8 +204,21 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -239,6 +252,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -279,7 +298,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -319,12 +338,15 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -607,7 +629,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="V19" sqref="V19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -676,43 +700,43 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="14.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="M2" s="17" t="s">
+      <c r="C2" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2" s="21" t="s">
         <v>3</v>
       </c>
       <c r="N2" s="14"/>
@@ -721,7 +745,7 @@
       <c r="Q2" s="15"/>
     </row>
     <row r="3" spans="1:17" ht="14.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="17" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="10" t="s">
@@ -746,7 +770,7 @@
       <c r="Q3" s="15"/>
     </row>
     <row r="4" spans="1:17" ht="14.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="17" t="s">
         <v>21</v>
       </c>
       <c r="B4" s="10" t="s">
@@ -771,12 +795,12 @@
       <c r="Q4" s="15"/>
     </row>
     <row r="5" spans="1:17" ht="14.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="18" t="s">
         <v>22</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="21" t="s">
         <v>3</v>
       </c>
       <c r="E5" s="2"/>
@@ -787,7 +811,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
-      <c r="M5" s="17" t="s">
+      <c r="M5" s="21" t="s">
         <v>3</v>
       </c>
       <c r="N5" s="14"/>
@@ -796,12 +820,12 @@
       <c r="Q5" s="15"/>
     </row>
     <row r="6" spans="1:17" ht="14.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="18" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="21" t="s">
         <v>3</v>
       </c>
       <c r="E6" s="2"/>
@@ -819,12 +843,12 @@
       <c r="Q6" s="15"/>
     </row>
     <row r="7" spans="1:17" ht="14.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
         <v>24</v>
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="21" t="s">
         <v>3</v>
       </c>
       <c r="E7" s="2"/>
@@ -842,12 +866,12 @@
       <c r="Q7" s="15"/>
     </row>
     <row r="8" spans="1:17" ht="14.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="18" t="s">
         <v>25</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="2"/>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="21" t="s">
         <v>3</v>
       </c>
       <c r="E8" s="2"/>
@@ -865,11 +889,11 @@
       <c r="Q8" s="15"/>
     </row>
     <row r="9" spans="1:17" ht="14.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="18" t="s">
         <v>26</v>
       </c>
       <c r="B9" s="9"/>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="21" t="s">
         <v>3</v>
       </c>
       <c r="D9" s="2"/>
@@ -888,11 +912,11 @@
       <c r="Q9" s="15"/>
     </row>
     <row r="10" spans="1:17" ht="14.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="18" t="s">
         <v>27</v>
       </c>
       <c r="B10" s="9"/>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="21" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="2"/>
@@ -911,11 +935,11 @@
       <c r="Q10" s="15"/>
     </row>
     <row r="11" spans="1:17" ht="14.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="18" t="s">
         <v>28</v>
       </c>
       <c r="B11" s="9"/>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="21" t="s">
         <v>3</v>
       </c>
       <c r="D11" s="2"/>
@@ -927,7 +951,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
-      <c r="M11" s="17" t="s">
+      <c r="M11" s="21" t="s">
         <v>3</v>
       </c>
       <c r="N11" s="14"/>
@@ -936,11 +960,11 @@
       <c r="Q11" s="15"/>
     </row>
     <row r="12" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="18" t="s">
         <v>29</v>
       </c>
       <c r="B12" s="9"/>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="21" t="s">
         <v>3</v>
       </c>
       <c r="D12" s="2"/>
@@ -952,7 +976,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
-      <c r="M12" s="17" t="s">
+      <c r="M12" s="21" t="s">
         <v>3</v>
       </c>
       <c r="N12" s="14"/>
@@ -961,7 +985,7 @@
       <c r="Q12" s="15"/>
     </row>
     <row r="13" spans="1:17" ht="14.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="18" t="s">
         <v>30</v>
       </c>
       <c r="B13" s="9"/>
@@ -969,7 +993,7 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="3" t="s">
+      <c r="G13" s="20" t="s">
         <v>3</v>
       </c>
       <c r="H13" s="2"/>
@@ -984,7 +1008,7 @@
       <c r="Q13" s="15"/>
     </row>
     <row r="14" spans="1:17" ht="14.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="18" t="s">
         <v>31</v>
       </c>
       <c r="B14" s="9"/>
@@ -1005,7 +1029,7 @@
       <c r="Q14" s="15"/>
     </row>
     <row r="15" spans="1:17" ht="14.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="18" t="s">
         <v>32</v>
       </c>
       <c r="B15" s="9"/>
@@ -1026,14 +1050,14 @@
       <c r="Q15" s="15"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="18" t="s">
         <v>33</v>
       </c>
       <c r="B16" s="9"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="21" t="s">
         <v>3</v>
       </c>
       <c r="G16" s="2"/>
@@ -1049,25 +1073,25 @@
       <c r="Q16" s="15"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="18" t="s">
         <v>34</v>
       </c>
       <c r="B17" s="9"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="21" t="s">
         <v>3</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
-      <c r="J17" s="3" t="s">
+      <c r="J17" s="21" t="s">
         <v>3</v>
       </c>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
-      <c r="M17" s="17" t="s">
+      <c r="M17" s="21" t="s">
         <v>3</v>
       </c>
       <c r="N17" s="14"/>
@@ -1076,7 +1100,7 @@
       <c r="Q17" s="15"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="18" t="s">
         <v>35</v>
       </c>
       <c r="B18" s="9"/>
@@ -1086,7 +1110,7 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
-      <c r="I18" s="3" t="s">
+      <c r="I18" s="21" t="s">
         <v>3</v>
       </c>
       <c r="J18" s="2"/>
@@ -1099,7 +1123,7 @@
       <c r="Q18" s="15"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="18" t="s">
         <v>36</v>
       </c>
       <c r="B19" s="9"/>
@@ -1109,7 +1133,7 @@
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
-      <c r="I19" s="3" t="s">
+      <c r="I19" s="21" t="s">
         <v>3</v>
       </c>
       <c r="J19" s="2"/>
@@ -1122,7 +1146,7 @@
       <c r="Q19" s="15"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="20" t="s">
+      <c r="A20" s="19" t="s">
         <v>37</v>
       </c>
       <c r="B20" s="9"/>
@@ -1134,11 +1158,11 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
-      <c r="K20" s="3" t="s">
+      <c r="K20" s="21" t="s">
         <v>3</v>
       </c>
       <c r="L20" s="3"/>
-      <c r="M20" s="17" t="s">
+      <c r="M20" s="21" t="s">
         <v>3</v>
       </c>
       <c r="N20" s="14"/>
@@ -1147,7 +1171,7 @@
       <c r="Q20" s="15"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="19" t="s">
+      <c r="A21" s="18" t="s">
         <v>38</v>
       </c>
       <c r="B21" s="9"/>
@@ -1156,7 +1180,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
-      <c r="H21" s="3" t="s">
+      <c r="H21" s="21" t="s">
         <v>3</v>
       </c>
       <c r="I21" s="2"/>
@@ -1170,7 +1194,7 @@
       <c r="Q21" s="15"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" s="19" t="s">
+      <c r="A22" s="18" t="s">
         <v>39</v>
       </c>
       <c r="B22" s="9"/>
@@ -1191,7 +1215,7 @@
       <c r="Q22" s="15"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" s="19" t="s">
+      <c r="A23" s="18" t="s">
         <v>40</v>
       </c>
       <c r="B23" s="9"/>
@@ -1204,7 +1228,7 @@
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
-      <c r="L23" s="3" t="s">
+      <c r="L23" s="21" t="s">
         <v>3</v>
       </c>
       <c r="M23" s="15"/>
@@ -1214,7 +1238,7 @@
       <c r="Q23" s="15"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="19" t="s">
+      <c r="A24" s="18" t="s">
         <v>41</v>
       </c>
       <c r="B24" s="9"/>
@@ -1235,7 +1259,7 @@
       <c r="Q24" s="15"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" s="19" t="s">
+      <c r="A25" s="18" t="s">
         <v>42</v>
       </c>
       <c r="B25" s="9"/>

</xml_diff>